<commit_message>
Libs für alle Sensoren
</commit_message>
<xml_diff>
--- a/docs/Labels.xlsx
+++ b/docs/Labels.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae4114ffef1ef242/Dokumente/Biodom Mini/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frank\Source\PlatformIO\biodom-mini\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{09783A56-710A-4773-B049-01A9C7A751A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D1F7D36-3430-4666-9702-C803EA34E27A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FF8F52-DE6A-456D-A157-9B5A76289FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="1688" windowWidth="16200" windowHeight="9990" activeTab="2" xr2:uid="{2302866B-0EA2-4005-A22C-9E69E28B23A5}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="3" xr2:uid="{2302866B-0EA2-4005-A22C-9E69E28B23A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Platine oben" sheetId="1" r:id="rId1"/>
     <sheet name="Platine rechts" sheetId="3" r:id="rId2"/>
     <sheet name="ESP-Prog" sheetId="4" r:id="rId3"/>
+    <sheet name="Anschlüsse" sheetId="5" r:id="rId4"/>
+    <sheet name="Tabelle3" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Power
 GND  3V3  5V  12V</t>
@@ -164,13 +166,46 @@
   </si>
   <si>
     <t xml:space="preserve">  G15</t>
+  </si>
+  <si>
+    <t>Bodentemp.</t>
+  </si>
+  <si>
+    <t>Luft</t>
+  </si>
+  <si>
+    <t>DC 12V</t>
+  </si>
+  <si>
+    <t>Wasserstand</t>
+  </si>
+  <si>
+    <t>Bodenfeuchte</t>
+  </si>
+  <si>
+    <t>Dunst</t>
+  </si>
+  <si>
+    <t>Pumpe</t>
+  </si>
+  <si>
+    <t>Lüfter</t>
+  </si>
+  <si>
+    <t>Heizer</t>
+  </si>
+  <si>
+    <t>Lampe 1</t>
+  </si>
+  <si>
+    <t>Lampe 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +227,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -201,7 +243,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -250,11 +292,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -280,9 +331,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -298,10 +376,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -685,7 +759,7 @@
   <dimension ref="A5:I7"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -754,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{747CFE7F-2E40-40F8-BA57-F7CB9455F68A}">
   <dimension ref="B2:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -773,7 +847,7 @@
       <c r="C2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="2:4" s="4" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C3" s="7"/>
@@ -786,7 +860,7 @@
       <c r="C4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="2:4" s="4" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C5" s="7"/>
@@ -799,7 +873,7 @@
       <c r="C6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="2:4" s="4" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C7" s="7"/>
@@ -812,7 +886,7 @@
       <c r="C8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="2:4" s="4" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C9" s="7"/>
@@ -825,7 +899,7 @@
       <c r="C10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="2:4" s="4" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C11" s="7"/>
@@ -838,7 +912,7 @@
       <c r="C12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="9"/>
+      <c r="D12" s="7"/>
     </row>
     <row r="13" spans="2:4" s="4" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C13" s="7"/>
@@ -851,7 +925,7 @@
       <c r="C14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="9"/>
+      <c r="D14" s="7"/>
     </row>
     <row r="15" spans="2:4" s="4" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C15" s="7"/>
@@ -864,7 +938,7 @@
       <c r="C16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="9"/>
+      <c r="D16" s="7"/>
     </row>
     <row r="17" spans="2:4" s="4" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C17" s="7"/>
@@ -877,7 +951,7 @@
       <c r="C18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="9"/>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="2:4" s="4" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C19" s="7"/>
@@ -890,7 +964,212 @@
       <c r="C20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="9"/>
+      <c r="D20" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F5515E-4454-4B6F-87AE-AA4DF1275C05}">
+  <dimension ref="B1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="10.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="7.59765625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="6.19921875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="7.59765625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="5.53125" style="18" customWidth="1"/>
+    <col min="6" max="6" width="6.19921875" style="18" customWidth="1"/>
+    <col min="7" max="7" width="5.59765625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="6.19921875" style="18" customWidth="1"/>
+    <col min="9" max="16384" width="10.6640625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="16"/>
+      <c r="H2" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="16"/>
+      <c r="H4" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" s="20" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="15"/>
+      <c r="C6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA14D7C-046A-4B5F-9182-9B43017A8B4A}">
+  <dimension ref="B1:J12"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="4.796875" customWidth="1"/>
+    <col min="2" max="2" width="2.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.06640625" customWidth="1"/>
+    <col min="4" max="4" width="2.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" customWidth="1"/>
+    <col min="6" max="6" width="2.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1328125" customWidth="1"/>
+    <col min="10" max="10" width="2.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="24.4" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:10" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="F2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="2:10" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="10"/>
+      <c r="F4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="2:10" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="11" spans="2:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="12" spans="2:10" ht="27" x14ac:dyDescent="0.45">
+      <c r="D12" s="9" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>